<commit_message>
added swell pedal support
</commit_message>
<xml_diff>
--- a/docs/MIDI_menuItems.xlsx
+++ b/docs/MIDI_menuItems.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
   <si>
     <t>Index #</t>
   </si>
@@ -575,6 +575,9 @@
   </si>
   <si>
     <t>setBtnMode</t>
+  </si>
+  <si>
+    <t>Swell CC</t>
   </si>
 </sst>
 </file>
@@ -1407,10 +1410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N70"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17:M20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,7 +1531,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A54" si="1">A2+1</f>
+        <f t="shared" ref="A3:A55" si="1">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1554,27 +1557,27 @@
         <v>97</v>
       </c>
       <c r="I3" s="43" t="str">
-        <f t="shared" ref="I3:I54" si="2">CONCATENATE("""",B3,""", ")</f>
+        <f t="shared" ref="I3:I55" si="2">CONCATENATE("""",B3,""", ")</f>
         <v xml:space="preserve">"Lower Channel", </v>
       </c>
       <c r="J3" s="44" t="str">
-        <f t="shared" ref="J3:J54" si="3">IF(G3="NULL",CONCATENATE(G3,", "),CONCATENATE("&amp;",G3,", "))</f>
+        <f t="shared" ref="J3:J55" si="3">IF(G3="NULL",CONCATENATE(G3,", "),CONCATENATE("&amp;",G3,", "))</f>
         <v xml:space="preserve">&amp;MenuValues[1], </v>
       </c>
       <c r="K3" s="44" t="str">
-        <f t="shared" ref="K3:K54" si="4">IF(H3="NULL",CONCATENATE(H3,", "),CONCATENATE("&amp;",H3,", "))</f>
+        <f t="shared" ref="K3:K55" si="4">IF(H3="NULL",CONCATENATE(H3,", "),CONCATENATE("&amp;",H3,", "))</f>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L3" s="40" t="str">
-        <f>CONCATENATE("  {",I3,C3,", ",J3,K3,D3,", ",E3,"},")</f>
+        <f t="shared" ref="L3:L35" si="5">CONCATENATE("  {",I3,C3,", ",J3,K3,D3,", ",E3,"},")</f>
         <v xml:space="preserve">  {"Lower Channel", m_lower_ch, &amp;MenuValues[1], NULL, 1, 16},</v>
       </c>
       <c r="M3" s="76" t="str">
-        <f t="shared" ref="M3:M54" si="5" xml:space="preserve"> CONCATENATE("  ",F3,",  // ",B3)</f>
+        <f t="shared" ref="M3:M55" si="6" xml:space="preserve"> CONCATENATE("  ",F3,",  // ",B3)</f>
         <v xml:space="preserve">  2,  // Lower Channel</v>
       </c>
       <c r="N3" s="53" t="str">
-        <f t="shared" ref="N3:N11" si="6">CONCATENATE("  ",C3,",")</f>
+        <f t="shared" ref="N3:N12" si="7">CONCATENATE("  ",C3,",")</f>
         <v xml:space="preserve">  m_lower_ch,</v>
       </c>
     </row>
@@ -1618,33 +1621,33 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L4" s="40" t="str">
-        <f>CONCATENATE("  {",I4,C4,", ",J4,K4,D4,", ",E4,"},")</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve">  {"Pedal Channel", m_pedal_ch, &amp;MenuValues[2], NULL, 1, 16},</v>
       </c>
       <c r="M4" s="76" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">  3,  // Pedal Channel</v>
       </c>
       <c r="N4" s="53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v xml:space="preserve">  m_pedal_ch,</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>60</v>
+      <c r="B5" s="20" t="s">
+        <v>185</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D5" s="20">
         <v>-1</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="20">
         <v>127</v>
       </c>
       <c r="F5" s="20">
@@ -1658,28 +1661,28 @@
         <v>97</v>
       </c>
       <c r="I5" s="43" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pitchwheel Pot", </v>
+        <f t="shared" ref="I5" si="8">CONCATENATE("""",B5,""", ")</f>
+        <v xml:space="preserve">"Swell CC", </v>
       </c>
       <c r="J5" s="44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="J5" si="9">IF(G5="NULL",CONCATENATE(G5,", "),CONCATENATE("&amp;",G5,", "))</f>
         <v xml:space="preserve">&amp;MenuValues[3], </v>
       </c>
       <c r="K5" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="K5" si="10">IF(H5="NULL",CONCATENATE(H5,", "),CONCATENATE("&amp;",H5,", "))</f>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L5" s="40" t="str">
-        <f>CONCATENATE("  {",I5,C5,", ",J5,K5,D5,", ",E5,"},")</f>
-        <v xml:space="preserve">  {"Pitchwheel Pot", m_pitchwheel, &amp;MenuValues[3], NULL, -1, 127},</v>
+        <f t="shared" ref="L5" si="11">CONCATENATE("  {",I5,C5,", ",J5,K5,D5,", ",E5,"},")</f>
+        <v xml:space="preserve">  {"Swell CC", m_swell, &amp;MenuValues[3], NULL, -1, 127},</v>
       </c>
       <c r="M5" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Pitchwheel Pot</v>
+        <f t="shared" ref="M5" si="12" xml:space="preserve"> CONCATENATE("  ",F5,",  // ",B5)</f>
+        <v xml:space="preserve">  -1,  // Swell CC</v>
       </c>
       <c r="N5" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  m_pitchwheel,</v>
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">  m_swell,</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1688,10 +1691,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="D6" s="20">
         <v>-1</v>
@@ -1711,78 +1714,79 @@
       </c>
       <c r="I6" s="43" t="str">
         <f t="shared" si="2"/>
+        <v xml:space="preserve">"Pitchwheel Pot", </v>
+      </c>
+      <c r="J6" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&amp;MenuValues[4], </v>
+      </c>
+      <c r="K6" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L6" s="40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pitchwheel Pot", m_pitchwheel, &amp;MenuValues[4], NULL, -1, 127},</v>
+      </c>
+      <c r="M6" s="76" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Pitchwheel Pot</v>
+      </c>
+      <c r="N6" s="53" t="str">
+        <f>CONCATENATE("  ",C6,",")</f>
+        <v xml:space="preserve">  m_pitchwheel,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="D7" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>127</v>
+      </c>
+      <c r="F7" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G7" s="29" t="str">
+        <f>CONCATENATE("MenuValues[",A7,"]")</f>
+        <v>MenuValues[5]</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I7" s="43" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">"Modulation Pot", </v>
       </c>
-      <c r="J6" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;MenuValues[4], </v>
-      </c>
-      <c r="K6" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L6" s="40" t="str">
-        <f>CONCATENATE("  {",I6,C6,", ",J6,K6,D6,", ",E6,"},")</f>
-        <v xml:space="preserve">  {"Modulation Pot", m_mod_pot, &amp;MenuValues[4], NULL, -1, 127},</v>
-      </c>
-      <c r="M6" s="76" t="str">
+      <c r="J7" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&amp;MenuValues[5], </v>
+      </c>
+      <c r="K7" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L7" s="40" t="str">
         <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Modulation Pot", m_mod_pot, &amp;MenuValues[5], NULL, -1, 127},</v>
+      </c>
+      <c r="M7" s="76" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">  -1,  // Modulation Pot</v>
       </c>
-      <c r="N6" s="53" t="str">
-        <f t="shared" si="6"/>
+      <c r="N7" s="53" t="str">
+        <f>CONCATENATE("  ",C7,",")</f>
         <v xml:space="preserve">  m_mod_pot,</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="20">
-        <v>-1</v>
-      </c>
-      <c r="E7" s="20">
-        <v>-1</v>
-      </c>
-      <c r="F7" s="20">
-        <v>-1</v>
-      </c>
-      <c r="G7" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H7" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="I7" s="43" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">"Keyboard", </v>
-      </c>
-      <c r="J7" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="K7" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L7" s="40" t="str">
-        <f>CONCATENATE("  {",I7,C7,", ",J7,K7,D7,", ",E7,"},")</f>
-        <v xml:space="preserve">  {"Keyboard", m_kbd_driver, NULL, NULL, -1, -1},</v>
-      </c>
-      <c r="M7" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Keyboard</v>
-      </c>
-      <c r="N7" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  m_kbd_driver,</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1791,10 +1795,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>172</v>
+        <v>112</v>
       </c>
       <c r="D8" s="20">
         <v>-1</v>
@@ -1813,7 +1817,7 @@
       </c>
       <c r="I8" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pot Assign", </v>
+        <v xml:space="preserve">"Keyboard", </v>
       </c>
       <c r="J8" s="44" t="str">
         <f t="shared" si="3"/>
@@ -1824,16 +1828,16 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L8" s="40" t="str">
-        <f>CONCATENATE("  {",I8,C8,", ",J8,K8,D8,", ",E8,"},")</f>
-        <v xml:space="preserve">  {"Pot Assign", m_pot_assign, NULL, NULL, -1, -1},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Keyboard", m_kbd_driver, NULL, NULL, -1, -1},</v>
       </c>
       <c r="M8" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Pot Assign</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Keyboard</v>
       </c>
       <c r="N8" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  m_pot_assign,</v>
+        <f>CONCATENATE("  ",C8,",")</f>
+        <v xml:space="preserve">  m_kbd_driver,</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1842,10 +1846,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D9" s="20">
         <v>-1</v>
@@ -1864,7 +1868,7 @@
       </c>
       <c r="I9" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Button Assign", </v>
+        <v xml:space="preserve">"Pot Assign", </v>
       </c>
       <c r="J9" s="44" t="str">
         <f t="shared" si="3"/>
@@ -1875,16 +1879,16 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L9" s="40" t="str">
-        <f>CONCATENATE("  {",I9,C9,", ",J9,K9,D9,", ",E9,"},")</f>
-        <v xml:space="preserve">  {"Button Assign", m_btn_assign, NULL, NULL, -1, -1},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pot Assign", m_pot_assign, NULL, NULL, -1, -1},</v>
       </c>
       <c r="M9" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Button Assign</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Pot Assign</v>
       </c>
       <c r="N9" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  m_btn_assign,</v>
+        <f>CONCATENATE("  ",C9,",")</f>
+        <v xml:space="preserve">  m_pot_assign,</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1893,100 +1897,100 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="20">
+        <v>-1</v>
+      </c>
+      <c r="F10" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="43" t="str">
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"Button Assign", </v>
+      </c>
+      <c r="J10" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="K10" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L10" s="40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Button Assign", m_btn_assign, NULL, NULL, -1, -1},</v>
+      </c>
+      <c r="M10" s="76" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Button Assign</v>
+      </c>
+      <c r="N10" s="53" t="str">
+        <f>CONCATENATE("  ",C10,",")</f>
+        <v xml:space="preserve">  m_btn_assign,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C11" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="D10" s="20">
-        <v>-1</v>
-      </c>
-      <c r="E10" s="20">
-        <v>-1</v>
-      </c>
-      <c r="F10" s="20">
-        <v>-1</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="I10" s="43" t="str">
+      <c r="D11" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E11" s="20">
+        <v>-1</v>
+      </c>
+      <c r="F11" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="43" t="str">
         <f t="shared" si="2"/>
         <v xml:space="preserve">"Button Mode", </v>
       </c>
-      <c r="J10" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="K10" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L10" s="40" t="str">
-        <f>CONCATENATE("  {",I10,C10,", ",J10,K10,D10,", ",E10,"},")</f>
+      <c r="J11" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="K11" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L11" s="40" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve">  {"Button Mode", m_btn_mode, NULL, NULL, -1, -1},</v>
       </c>
-      <c r="M10" s="76" t="str">
-        <f t="shared" si="5"/>
+      <c r="M11" s="76" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">  -1,  // Button Mode</v>
       </c>
-      <c r="N10" s="53" t="str">
-        <f t="shared" si="6"/>
+      <c r="N11" s="53" t="str">
+        <f>CONCATENATE("  ",C11,",")</f>
         <v xml:space="preserve">  m_btn_mode,</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D11" s="20">
-        <v>-1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F11" s="20">
-        <v>-1</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="43" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">"End", </v>
-      </c>
-      <c r="J11" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="K11" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L11" s="40" t="str">
-        <f>CONCATENATE("  {",I11,C11,", ",J11,K11,D11,", ",E11,"},")</f>
-        <v xml:space="preserve">  {"End", m_main_end, NULL, NULL, -1, -1},</v>
-      </c>
-      <c r="M11" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // End</v>
-      </c>
-      <c r="N11" s="53" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">  m_main_end,</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1994,50 +1998,50 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>9</v>
+      <c r="B12" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
       <c r="D12" s="20">
         <v>-1</v>
       </c>
-      <c r="E12" s="20">
-        <v>127</v>
+      <c r="E12" s="1">
+        <v>-1</v>
       </c>
       <c r="F12" s="20">
         <v>-1</v>
       </c>
-      <c r="G12" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A12,"]")</f>
-        <v>MenuValues[10]</v>
+      <c r="G12" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="H12" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I12" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pot 1 CC", </v>
+        <v xml:space="preserve">"End", </v>
       </c>
       <c r="J12" s="44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;MenuValues[10], </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="K12" s="44" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L12" s="40" t="str">
-        <f>CONCATENATE("  {",I12,C12,", ",J12,K12,D12,", ",E12,"},")</f>
-        <v xml:space="preserve">  {"Pot 1 CC", m_pot_assign, &amp;MenuValues[10], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"End", m_main_end, NULL, NULL, -1, -1},</v>
       </c>
       <c r="M12" s="76" t="str">
-        <f xml:space="preserve"> CONCATENATE("  ",F12,",  // ",B12)</f>
-        <v xml:space="preserve">  -1,  // Pot 1 CC</v>
-      </c>
-      <c r="N12" s="53" t="s">
-        <v>159</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // End</v>
+      </c>
+      <c r="N12" s="53" t="str">
+        <f>CONCATENATE("  ",C12,",")</f>
+        <v xml:space="preserve">  m_main_end,</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -2045,8 +2049,8 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
+      <c r="B13" s="14" t="s">
+        <v>9</v>
       </c>
       <c r="C13" s="20" t="s">
         <v>172</v>
@@ -2069,7 +2073,7 @@
       </c>
       <c r="I13" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pot 2 CC", </v>
+        <v xml:space="preserve">"Pot 1 CC", </v>
       </c>
       <c r="J13" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2080,14 +2084,16 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L13" s="40" t="str">
-        <f>CONCATENATE("  {",I13,C13,", ",J13,K13,D13,", ",E13,"},")</f>
-        <v xml:space="preserve">  {"Pot 2 CC", m_pot_assign, &amp;MenuValues[11], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pot 1 CC", m_pot_assign, &amp;MenuValues[11], NULL, -1, 127},</v>
       </c>
       <c r="M13" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Pot 2 CC</v>
-      </c>
-      <c r="N13" s="53"/>
+        <f xml:space="preserve"> CONCATENATE("  ",F13,",  // ",B13)</f>
+        <v xml:space="preserve">  -1,  // Pot 1 CC</v>
+      </c>
+      <c r="N13" s="53" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
@@ -2095,7 +2101,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C14" s="20" t="s">
         <v>172</v>
@@ -2118,7 +2124,7 @@
       </c>
       <c r="I14" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pot 3 CC", </v>
+        <v xml:space="preserve">"Pot 2 CC", </v>
       </c>
       <c r="J14" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2129,12 +2135,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L14" s="40" t="str">
-        <f>CONCATENATE("  {",I14,C14,", ",J14,K14,D14,", ",E14,"},")</f>
-        <v xml:space="preserve">  {"Pot 3 CC", m_pot_assign, &amp;MenuValues[12], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pot 2 CC", m_pot_assign, &amp;MenuValues[12], NULL, -1, 127},</v>
       </c>
       <c r="M14" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Pot 3 CC</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Pot 2 CC</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2143,7 +2149,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="20" t="s">
         <v>172</v>
@@ -2166,7 +2172,7 @@
       </c>
       <c r="I15" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Pot 4 CC", </v>
+        <v xml:space="preserve">"Pot 3 CC", </v>
       </c>
       <c r="J15" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2177,119 +2183,118 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L15" s="40" t="str">
-        <f>CONCATENATE("  {",I15,C15,", ",J15,K15,D15,", ",E15,"},")</f>
-        <v xml:space="preserve">  {"Pot 4 CC", m_pot_assign, &amp;MenuValues[13], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pot 3 CC", m_pot_assign, &amp;MenuValues[13], NULL, -1, 127},</v>
       </c>
       <c r="M15" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Pot 4 CC</v>
-      </c>
-      <c r="N15" s="7"/>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Pot 3 CC</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>175</v>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="D16" s="61">
-        <v>-1</v>
-      </c>
-      <c r="E16" s="61">
-        <v>-1</v>
-      </c>
-      <c r="F16" s="61">
-        <v>-1</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>97</v>
+      <c r="D16" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E16" s="20">
+        <v>127</v>
+      </c>
+      <c r="F16" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G16" s="29" t="str">
+        <f>CONCATENATE("MenuValues[",A16,"]")</f>
+        <v>MenuValues[14]</v>
       </c>
       <c r="H16" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I16" s="43" t="str">
         <f t="shared" si="2"/>
+        <v xml:space="preserve">"Pot 4 CC", </v>
+      </c>
+      <c r="J16" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">&amp;MenuValues[14], </v>
+      </c>
+      <c r="K16" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L16" s="40" t="str">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Pot 4 CC", m_pot_assign, &amp;MenuValues[14], NULL, -1, 127},</v>
+      </c>
+      <c r="M16" s="76" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Pot 4 CC</v>
+      </c>
+      <c r="N16" s="7"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="D17" s="61">
+        <v>-1</v>
+      </c>
+      <c r="E17" s="61">
+        <v>-1</v>
+      </c>
+      <c r="F17" s="61">
+        <v>-1</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" s="43" t="str">
+        <f t="shared" si="2"/>
         <v xml:space="preserve">"Pot CC", </v>
       </c>
-      <c r="J16" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="K16" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L16" s="40" t="str">
-        <f>CONCATENATE("  {",I16,C16,", ",J16,K16,D16,", ",E16,"},")</f>
+      <c r="J17" s="44" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="K17" s="44" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L17" s="40" t="str">
+        <f t="shared" si="5"/>
         <v xml:space="preserve">  {"Pot CC", m_pot_assign, NULL, NULL, -1, -1},</v>
       </c>
-      <c r="M16" s="76" t="str">
-        <f t="shared" si="5"/>
+      <c r="M17" s="76" t="str">
+        <f t="shared" si="6"/>
         <v xml:space="preserve">  -1,  // Pot CC</v>
       </c>
-      <c r="N16" s="7"/>
-    </row>
-    <row r="17" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="14" t="s">
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D17" s="20">
-        <v>-1</v>
-      </c>
-      <c r="E17" s="20">
-        <v>127</v>
-      </c>
-      <c r="F17" s="20">
-        <v>-1</v>
-      </c>
-      <c r="G17" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A17,"]")</f>
-        <v>MenuValues[15]</v>
-      </c>
-      <c r="H17" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="I17" s="43" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 1 CC/Prg", </v>
-      </c>
-      <c r="J17" s="44" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;MenuValues[15], </v>
-      </c>
-      <c r="K17" s="44" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L17" s="40" t="str">
-        <f>CONCATENATE("  {",I17,C17,", ",J17,K17,D17,", ",E17,"},")</f>
-        <v xml:space="preserve">  {"Btn 1 CC/Prg", m_btn_assign, &amp;MenuValues[15], NULL, -1, 127},</v>
-      </c>
-      <c r="M17" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 1 CC/Prg</v>
-      </c>
-      <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
-        <f t="shared" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>173</v>
@@ -2304,7 +2309,7 @@
         <v>-1</v>
       </c>
       <c r="G18" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A18,"]")</f>
+        <f t="shared" ref="G18:G33" si="13">CONCATENATE("MenuValues[",A18,"]")</f>
         <v>MenuValues[16]</v>
       </c>
       <c r="H18" s="29" t="s">
@@ -2312,7 +2317,7 @@
       </c>
       <c r="I18" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 2 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 1 CC/Prg", </v>
       </c>
       <c r="J18" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2323,12 +2328,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L18" s="40" t="str">
-        <f>CONCATENATE("  {",I18,C18,", ",J18,K18,D18,", ",E18,"},")</f>
-        <v xml:space="preserve">  {"Btn 2 CC/Prg", m_btn_assign, &amp;MenuValues[16], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 1 CC/Prg", m_btn_assign, &amp;MenuValues[16], NULL, -1, 127},</v>
       </c>
       <c r="M18" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 2 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 1 CC/Prg</v>
       </c>
       <c r="N18" s="7"/>
     </row>
@@ -2338,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>173</v>
@@ -2353,7 +2358,7 @@
         <v>-1</v>
       </c>
       <c r="G19" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A19,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[17]</v>
       </c>
       <c r="H19" s="29" t="s">
@@ -2361,7 +2366,7 @@
       </c>
       <c r="I19" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 3 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 2 CC/Prg", </v>
       </c>
       <c r="J19" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2372,12 +2377,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L19" s="40" t="str">
-        <f>CONCATENATE("  {",I19,C19,", ",J19,K19,D19,", ",E19,"},")</f>
-        <v xml:space="preserve">  {"Btn 3 CC/Prg", m_btn_assign, &amp;MenuValues[17], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 2 CC/Prg", m_btn_assign, &amp;MenuValues[17], NULL, -1, 127},</v>
       </c>
       <c r="M19" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 3 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 2 CC/Prg</v>
       </c>
       <c r="N19" s="7"/>
     </row>
@@ -2387,7 +2392,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>173</v>
@@ -2402,7 +2407,7 @@
         <v>-1</v>
       </c>
       <c r="G20" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A20,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[18]</v>
       </c>
       <c r="H20" s="29" t="s">
@@ -2410,7 +2415,7 @@
       </c>
       <c r="I20" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 4 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 3 CC/Prg", </v>
       </c>
       <c r="J20" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2421,12 +2426,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L20" s="40" t="str">
-        <f>CONCATENATE("  {",I20,C20,", ",J20,K20,D20,", ",E20,"},")</f>
-        <v xml:space="preserve">  {"Btn 4 CC/Prg", m_btn_assign, &amp;MenuValues[18], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 3 CC/Prg", m_btn_assign, &amp;MenuValues[18], NULL, -1, 127},</v>
       </c>
       <c r="M20" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 4 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 3 CC/Prg</v>
       </c>
       <c r="N20" s="7"/>
     </row>
@@ -2436,7 +2441,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>173</v>
@@ -2451,7 +2456,7 @@
         <v>-1</v>
       </c>
       <c r="G21" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A21,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[19]</v>
       </c>
       <c r="H21" s="29" t="s">
@@ -2459,7 +2464,7 @@
       </c>
       <c r="I21" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 5 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 4 CC/Prg", </v>
       </c>
       <c r="J21" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2470,12 +2475,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L21" s="40" t="str">
-        <f>CONCATENATE("  {",I21,C21,", ",J21,K21,D21,", ",E21,"},")</f>
-        <v xml:space="preserve">  {"Btn 5 CC/Prg", m_btn_assign, &amp;MenuValues[19], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 4 CC/Prg", m_btn_assign, &amp;MenuValues[19], NULL, -1, 127},</v>
       </c>
       <c r="M21" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 5 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 4 CC/Prg</v>
       </c>
       <c r="N21" s="7"/>
     </row>
@@ -2485,7 +2490,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>173</v>
@@ -2500,7 +2505,7 @@
         <v>-1</v>
       </c>
       <c r="G22" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A22,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[20]</v>
       </c>
       <c r="H22" s="29" t="s">
@@ -2508,7 +2513,7 @@
       </c>
       <c r="I22" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 6 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 5 CC/Prg", </v>
       </c>
       <c r="J22" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2519,12 +2524,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L22" s="40" t="str">
-        <f>CONCATENATE("  {",I22,C22,", ",J22,K22,D22,", ",E22,"},")</f>
-        <v xml:space="preserve">  {"Btn 6 CC/Prg", m_btn_assign, &amp;MenuValues[20], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 5 CC/Prg", m_btn_assign, &amp;MenuValues[20], NULL, -1, 127},</v>
       </c>
       <c r="M22" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 6 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 5 CC/Prg</v>
       </c>
       <c r="N22" s="7"/>
     </row>
@@ -2534,7 +2539,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>173</v>
@@ -2549,7 +2554,7 @@
         <v>-1</v>
       </c>
       <c r="G23" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A23,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[21]</v>
       </c>
       <c r="H23" s="29" t="s">
@@ -2557,7 +2562,7 @@
       </c>
       <c r="I23" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 7 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 6 CC/Prg", </v>
       </c>
       <c r="J23" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2568,12 +2573,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L23" s="40" t="str">
-        <f>CONCATENATE("  {",I23,C23,", ",J23,K23,D23,", ",E23,"},")</f>
-        <v xml:space="preserve">  {"Btn 7 CC/Prg", m_btn_assign, &amp;MenuValues[21], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 6 CC/Prg", m_btn_assign, &amp;MenuValues[21], NULL, -1, 127},</v>
       </c>
       <c r="M23" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 7 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 6 CC/Prg</v>
       </c>
       <c r="N23" s="7"/>
     </row>
@@ -2583,7 +2588,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" s="20" t="s">
         <v>173</v>
@@ -2598,7 +2603,7 @@
         <v>-1</v>
       </c>
       <c r="G24" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A24,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[22]</v>
       </c>
       <c r="H24" s="29" t="s">
@@ -2606,7 +2611,7 @@
       </c>
       <c r="I24" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 8 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 7 CC/Prg", </v>
       </c>
       <c r="J24" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2617,14 +2622,14 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L24" s="40" t="str">
-        <f>CONCATENATE("  {",I24,C24,", ",J24,K24,D24,", ",E24,"},")</f>
-        <v xml:space="preserve">  {"Btn 8 CC/Prg", m_btn_assign, &amp;MenuValues[22], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 7 CC/Prg", m_btn_assign, &amp;MenuValues[22], NULL, -1, 127},</v>
       </c>
       <c r="M24" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 8 CC/Prg</v>
-      </c>
-      <c r="N24" s="11"/>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 7 CC/Prg</v>
+      </c>
+      <c r="N24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
@@ -2632,7 +2637,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>173</v>
@@ -2647,7 +2652,7 @@
         <v>-1</v>
       </c>
       <c r="G25" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A25,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[23]</v>
       </c>
       <c r="H25" s="29" t="s">
@@ -2655,7 +2660,7 @@
       </c>
       <c r="I25" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 9 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 8 CC/Prg", </v>
       </c>
       <c r="J25" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2666,12 +2671,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L25" s="40" t="str">
-        <f>CONCATENATE("  {",I25,C25,", ",J25,K25,D25,", ",E25,"},")</f>
-        <v xml:space="preserve">  {"Btn 9 CC/Prg", m_btn_assign, &amp;MenuValues[23], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 8 CC/Prg", m_btn_assign, &amp;MenuValues[23], NULL, -1, 127},</v>
       </c>
       <c r="M25" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 9 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 8 CC/Prg</v>
       </c>
       <c r="N25" s="11"/>
     </row>
@@ -2681,7 +2686,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>173</v>
@@ -2696,7 +2701,7 @@
         <v>-1</v>
       </c>
       <c r="G26" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A26,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[24]</v>
       </c>
       <c r="H26" s="29" t="s">
@@ -2704,7 +2709,7 @@
       </c>
       <c r="I26" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 10 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 9 CC/Prg", </v>
       </c>
       <c r="J26" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2715,12 +2720,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L26" s="40" t="str">
-        <f>CONCATENATE("  {",I26,C26,", ",J26,K26,D26,", ",E26,"},")</f>
-        <v xml:space="preserve">  {"Btn 10 CC/Prg", m_btn_assign, &amp;MenuValues[24], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 9 CC/Prg", m_btn_assign, &amp;MenuValues[24], NULL, -1, 127},</v>
       </c>
       <c r="M26" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 10 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 9 CC/Prg</v>
       </c>
       <c r="N26" s="11"/>
     </row>
@@ -2730,7 +2735,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>173</v>
@@ -2745,7 +2750,7 @@
         <v>-1</v>
       </c>
       <c r="G27" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A27,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[25]</v>
       </c>
       <c r="H27" s="29" t="s">
@@ -2753,7 +2758,7 @@
       </c>
       <c r="I27" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 11 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 10 CC/Prg", </v>
       </c>
       <c r="J27" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2764,12 +2769,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L27" s="40" t="str">
-        <f>CONCATENATE("  {",I27,C27,", ",J27,K27,D27,", ",E27,"},")</f>
-        <v xml:space="preserve">  {"Btn 11 CC/Prg", m_btn_assign, &amp;MenuValues[25], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 10 CC/Prg", m_btn_assign, &amp;MenuValues[25], NULL, -1, 127},</v>
       </c>
       <c r="M27" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 11 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 10 CC/Prg</v>
       </c>
       <c r="N27" s="11"/>
     </row>
@@ -2779,7 +2784,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>173</v>
@@ -2794,7 +2799,7 @@
         <v>-1</v>
       </c>
       <c r="G28" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A28,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[26]</v>
       </c>
       <c r="H28" s="29" t="s">
@@ -2802,7 +2807,7 @@
       </c>
       <c r="I28" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 12 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 11 CC/Prg", </v>
       </c>
       <c r="J28" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2813,12 +2818,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L28" s="40" t="str">
-        <f>CONCATENATE("  {",I28,C28,", ",J28,K28,D28,", ",E28,"},")</f>
-        <v xml:space="preserve">  {"Btn 12 CC/Prg", m_btn_assign, &amp;MenuValues[26], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 11 CC/Prg", m_btn_assign, &amp;MenuValues[26], NULL, -1, 127},</v>
       </c>
       <c r="M28" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 12 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 11 CC/Prg</v>
       </c>
       <c r="N28" s="11"/>
     </row>
@@ -2828,7 +2833,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>173</v>
@@ -2843,7 +2848,7 @@
         <v>-1</v>
       </c>
       <c r="G29" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A29,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[27]</v>
       </c>
       <c r="H29" s="29" t="s">
@@ -2851,7 +2856,7 @@
       </c>
       <c r="I29" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 13 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 12 CC/Prg", </v>
       </c>
       <c r="J29" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2862,12 +2867,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L29" s="40" t="str">
-        <f>CONCATENATE("  {",I29,C29,", ",J29,K29,D29,", ",E29,"},")</f>
-        <v xml:space="preserve">  {"Btn 13 CC/Prg", m_btn_assign, &amp;MenuValues[27], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 12 CC/Prg", m_btn_assign, &amp;MenuValues[27], NULL, -1, 127},</v>
       </c>
       <c r="M29" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 13 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 12 CC/Prg</v>
       </c>
       <c r="N29" s="11"/>
     </row>
@@ -2877,7 +2882,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>173</v>
@@ -2892,7 +2897,7 @@
         <v>-1</v>
       </c>
       <c r="G30" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A30,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[28]</v>
       </c>
       <c r="H30" s="29" t="s">
@@ -2900,7 +2905,7 @@
       </c>
       <c r="I30" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 14 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 13 CC/Prg", </v>
       </c>
       <c r="J30" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2911,12 +2916,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L30" s="40" t="str">
-        <f>CONCATENATE("  {",I30,C30,", ",J30,K30,D30,", ",E30,"},")</f>
-        <v xml:space="preserve">  {"Btn 14 CC/Prg", m_btn_assign, &amp;MenuValues[28], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 13 CC/Prg", m_btn_assign, &amp;MenuValues[28], NULL, -1, 127},</v>
       </c>
       <c r="M30" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 14 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 13 CC/Prg</v>
       </c>
       <c r="N30" s="11"/>
     </row>
@@ -2926,7 +2931,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>173</v>
@@ -2941,7 +2946,7 @@
         <v>-1</v>
       </c>
       <c r="G31" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A31,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[29]</v>
       </c>
       <c r="H31" s="29" t="s">
@@ -2949,7 +2954,7 @@
       </c>
       <c r="I31" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 15 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 14 CC/Prg", </v>
       </c>
       <c r="J31" s="44" t="str">
         <f t="shared" si="3"/>
@@ -2960,12 +2965,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L31" s="40" t="str">
-        <f>CONCATENATE("  {",I31,C31,", ",J31,K31,D31,", ",E31,"},")</f>
-        <v xml:space="preserve">  {"Btn 15 CC/Prg", m_btn_assign, &amp;MenuValues[29], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 14 CC/Prg", m_btn_assign, &amp;MenuValues[29], NULL, -1, 127},</v>
       </c>
       <c r="M31" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 15 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 14 CC/Prg</v>
       </c>
       <c r="N31" s="11"/>
     </row>
@@ -2975,7 +2980,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>173</v>
@@ -2990,7 +2995,7 @@
         <v>-1</v>
       </c>
       <c r="G32" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A32,"]")</f>
+        <f t="shared" si="13"/>
         <v>MenuValues[30]</v>
       </c>
       <c r="H32" s="29" t="s">
@@ -2998,7 +3003,7 @@
       </c>
       <c r="I32" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 16 CC/Prg", </v>
+        <v xml:space="preserve">"Btn 15 CC/Prg", </v>
       </c>
       <c r="J32" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3009,12 +3014,12 @@
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L32" s="40" t="str">
-        <f>CONCATENATE("  {",I32,C32,", ",J32,K32,D32,", ",E32,"},")</f>
-        <v xml:space="preserve">  {"Btn 16 CC/Prg", m_btn_assign, &amp;MenuValues[30], NULL, -1, 127},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 15 CC/Prg", m_btn_assign, &amp;MenuValues[30], NULL, -1, 127},</v>
       </c>
       <c r="M32" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn 16 CC/Prg</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 15 CC/Prg</v>
       </c>
       <c r="N32" s="11"/>
     </row>
@@ -3023,46 +3028,47 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B33" s="13" t="s">
-        <v>176</v>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="D33" s="61">
-        <v>-1</v>
-      </c>
-      <c r="E33" s="61">
-        <v>-1</v>
-      </c>
-      <c r="F33" s="61">
-        <v>-1</v>
-      </c>
-      <c r="G33" s="29" t="s">
-        <v>97</v>
+      <c r="D33" s="20">
+        <v>-1</v>
+      </c>
+      <c r="E33" s="20">
+        <v>127</v>
+      </c>
+      <c r="F33" s="20">
+        <v>-1</v>
+      </c>
+      <c r="G33" s="29" t="str">
+        <f t="shared" si="13"/>
+        <v>MenuValues[31]</v>
       </c>
       <c r="H33" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I33" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn CC", </v>
+        <v xml:space="preserve">"Btn 16 CC/Prg", </v>
       </c>
       <c r="J33" s="44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
+        <v xml:space="preserve">&amp;MenuValues[31], </v>
       </c>
       <c r="K33" s="44" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L33" s="40" t="str">
-        <f>CONCATENATE("  {",I33,C33,", ",J33,K33,D33,", ",E33,"},")</f>
-        <v xml:space="preserve">  {"Btn CC", m_btn_assign, NULL, NULL, -1, -1},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 16 CC/Prg", m_btn_assign, &amp;MenuValues[31], NULL, -1, 127},</v>
       </c>
       <c r="M33" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn CC</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn 16 CC/Prg</v>
       </c>
       <c r="N33" s="11"/>
     </row>
@@ -3071,47 +3077,46 @@
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>26</v>
+      <c r="B34" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D34" s="20">
-        <v>0</v>
-      </c>
-      <c r="E34" s="20">
-        <v>3</v>
-      </c>
-      <c r="F34" s="20">
-        <v>0</v>
-      </c>
-      <c r="G34" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A34,"]")</f>
-        <v>MenuValues[32]</v>
+        <v>173</v>
+      </c>
+      <c r="D34" s="61">
+        <v>-1</v>
+      </c>
+      <c r="E34" s="61">
+        <v>-1</v>
+      </c>
+      <c r="F34" s="61">
+        <v>-1</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="H34" s="29" t="s">
-        <v>184</v>
+        <v>97</v>
       </c>
       <c r="I34" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 1 Mode", </v>
+        <v xml:space="preserve">"Btn CC", </v>
       </c>
       <c r="J34" s="44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;MenuValues[32], </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="K34" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">&amp;setBtnMode, </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L34" s="40" t="str">
-        <f>CONCATENATE("  {",I34,C34,", ",J34,K34,D34,", ",E34,"},")</f>
-        <v xml:space="preserve">  {"Btn 1 Mode", m_btn_mode, &amp;MenuValues[32], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn CC", m_btn_assign, NULL, NULL, -1, -1},</v>
       </c>
       <c r="M34" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 1 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn CC</v>
       </c>
       <c r="N34" s="11"/>
     </row>
@@ -3120,8 +3125,8 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>27</v>
+      <c r="B35" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="C35" s="20" t="s">
         <v>174</v>
@@ -3136,7 +3141,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A35,"]")</f>
+        <f t="shared" ref="G35:G50" si="14">CONCATENATE("MenuValues[",A35,"]")</f>
         <v>MenuValues[33]</v>
       </c>
       <c r="H35" s="29" t="s">
@@ -3144,7 +3149,7 @@
       </c>
       <c r="I35" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 2 Mode", </v>
+        <v xml:space="preserve">"Btn 1 Mode", </v>
       </c>
       <c r="J35" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3155,12 +3160,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L35" s="40" t="str">
-        <f>CONCATENATE("  {",I35,C35,", ",J35,K35,D35,", ",E35,"},")</f>
-        <v xml:space="preserve">  {"Btn 2 Mode", m_btn_mode, &amp;MenuValues[33], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  {"Btn 1 Mode", m_btn_mode, &amp;MenuValues[33], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M35" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 2 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 1 Mode</v>
       </c>
       <c r="N35" s="11"/>
     </row>
@@ -3170,7 +3175,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="20" t="s">
         <v>174</v>
@@ -3185,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="G36" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A36,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[34]</v>
       </c>
       <c r="H36" s="29" t="s">
@@ -3193,7 +3198,7 @@
       </c>
       <c r="I36" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 3 Mode", </v>
+        <v xml:space="preserve">"Btn 2 Mode", </v>
       </c>
       <c r="J36" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3204,12 +3209,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L36" s="40" t="str">
-        <f>CONCATENATE("  {",I36,C36,", ",J36,K36,D36,", ",E36,"},")</f>
-        <v xml:space="preserve">  {"Btn 3 Mode", m_btn_mode, &amp;MenuValues[34], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" ref="L36:L67" si="15">CONCATENATE("  {",I36,C36,", ",J36,K36,D36,", ",E36,"},")</f>
+        <v xml:space="preserve">  {"Btn 2 Mode", m_btn_mode, &amp;MenuValues[34], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M36" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 3 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 2 Mode</v>
       </c>
       <c r="N36" s="11"/>
     </row>
@@ -3219,7 +3224,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="20" t="s">
         <v>174</v>
@@ -3234,7 +3239,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A37,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[35]</v>
       </c>
       <c r="H37" s="29" t="s">
@@ -3242,7 +3247,7 @@
       </c>
       <c r="I37" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 4 Mode", </v>
+        <v xml:space="preserve">"Btn 3 Mode", </v>
       </c>
       <c r="J37" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3253,12 +3258,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L37" s="40" t="str">
-        <f>CONCATENATE("  {",I37,C37,", ",J37,K37,D37,", ",E37,"},")</f>
-        <v xml:space="preserve">  {"Btn 4 Mode", m_btn_mode, &amp;MenuValues[35], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 3 Mode", m_btn_mode, &amp;MenuValues[35], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M37" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 4 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 3 Mode</v>
       </c>
       <c r="N37" s="11"/>
     </row>
@@ -3268,7 +3273,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="20" t="s">
         <v>174</v>
@@ -3283,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="G38" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A38,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[36]</v>
       </c>
       <c r="H38" s="29" t="s">
@@ -3291,7 +3296,7 @@
       </c>
       <c r="I38" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 5 Mode", </v>
+        <v xml:space="preserve">"Btn 4 Mode", </v>
       </c>
       <c r="J38" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3302,12 +3307,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L38" s="40" t="str">
-        <f>CONCATENATE("  {",I38,C38,", ",J38,K38,D38,", ",E38,"},")</f>
-        <v xml:space="preserve">  {"Btn 5 Mode", m_btn_mode, &amp;MenuValues[36], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 4 Mode", m_btn_mode, &amp;MenuValues[36], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M38" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 5 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 4 Mode</v>
       </c>
       <c r="N38" s="11"/>
     </row>
@@ -3317,7 +3322,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>174</v>
@@ -3332,7 +3337,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A39,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[37]</v>
       </c>
       <c r="H39" s="29" t="s">
@@ -3340,7 +3345,7 @@
       </c>
       <c r="I39" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 6 Mode", </v>
+        <v xml:space="preserve">"Btn 5 Mode", </v>
       </c>
       <c r="J39" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3351,12 +3356,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L39" s="40" t="str">
-        <f>CONCATENATE("  {",I39,C39,", ",J39,K39,D39,", ",E39,"},")</f>
-        <v xml:space="preserve">  {"Btn 6 Mode", m_btn_mode, &amp;MenuValues[37], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 5 Mode", m_btn_mode, &amp;MenuValues[37], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M39" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 6 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 5 Mode</v>
       </c>
       <c r="N39" s="11"/>
     </row>
@@ -3366,7 +3371,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="20" t="s">
         <v>174</v>
@@ -3381,7 +3386,7 @@
         <v>0</v>
       </c>
       <c r="G40" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A40,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[38]</v>
       </c>
       <c r="H40" s="29" t="s">
@@ -3389,7 +3394,7 @@
       </c>
       <c r="I40" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 7 Mode", </v>
+        <v xml:space="preserve">"Btn 6 Mode", </v>
       </c>
       <c r="J40" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3400,12 +3405,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L40" s="40" t="str">
-        <f>CONCATENATE("  {",I40,C40,", ",J40,K40,D40,", ",E40,"},")</f>
-        <v xml:space="preserve">  {"Btn 7 Mode", m_btn_mode, &amp;MenuValues[38], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 6 Mode", m_btn_mode, &amp;MenuValues[38], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M40" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 7 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 6 Mode</v>
       </c>
       <c r="N40" s="11"/>
     </row>
@@ -3415,7 +3420,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="20" t="s">
         <v>174</v>
@@ -3430,7 +3435,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A41,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[39]</v>
       </c>
       <c r="H41" s="29" t="s">
@@ -3438,7 +3443,7 @@
       </c>
       <c r="I41" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 8 Mode", </v>
+        <v xml:space="preserve">"Btn 7 Mode", </v>
       </c>
       <c r="J41" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3449,12 +3454,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L41" s="40" t="str">
-        <f>CONCATENATE("  {",I41,C41,", ",J41,K41,D41,", ",E41,"},")</f>
-        <v xml:space="preserve">  {"Btn 8 Mode", m_btn_mode, &amp;MenuValues[39], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 7 Mode", m_btn_mode, &amp;MenuValues[39], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M41" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 8 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 7 Mode</v>
       </c>
       <c r="N41" s="11"/>
     </row>
@@ -3464,7 +3469,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="20" t="s">
         <v>174</v>
@@ -3479,7 +3484,7 @@
         <v>0</v>
       </c>
       <c r="G42" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A42,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[40]</v>
       </c>
       <c r="H42" s="29" t="s">
@@ -3487,7 +3492,7 @@
       </c>
       <c r="I42" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 9 Mode", </v>
+        <v xml:space="preserve">"Btn 8 Mode", </v>
       </c>
       <c r="J42" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3498,12 +3503,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L42" s="40" t="str">
-        <f>CONCATENATE("  {",I42,C42,", ",J42,K42,D42,", ",E42,"},")</f>
-        <v xml:space="preserve">  {"Btn 9 Mode", m_btn_mode, &amp;MenuValues[40], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 8 Mode", m_btn_mode, &amp;MenuValues[40], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M42" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 9 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 8 Mode</v>
       </c>
       <c r="N42" s="11"/>
     </row>
@@ -3513,7 +3518,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="20" t="s">
         <v>174</v>
@@ -3528,7 +3533,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A43,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[41]</v>
       </c>
       <c r="H43" s="29" t="s">
@@ -3536,7 +3541,7 @@
       </c>
       <c r="I43" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 10 Mode", </v>
+        <v xml:space="preserve">"Btn 9 Mode", </v>
       </c>
       <c r="J43" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3547,12 +3552,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L43" s="40" t="str">
-        <f>CONCATENATE("  {",I43,C43,", ",J43,K43,D43,", ",E43,"},")</f>
-        <v xml:space="preserve">  {"Btn 10 Mode", m_btn_mode, &amp;MenuValues[41], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 9 Mode", m_btn_mode, &amp;MenuValues[41], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M43" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 10 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 9 Mode</v>
       </c>
       <c r="N43" s="11"/>
     </row>
@@ -3562,7 +3567,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C44" s="20" t="s">
         <v>174</v>
@@ -3577,7 +3582,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A44,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[42]</v>
       </c>
       <c r="H44" s="29" t="s">
@@ -3585,7 +3590,7 @@
       </c>
       <c r="I44" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 11 Mode", </v>
+        <v xml:space="preserve">"Btn 10 Mode", </v>
       </c>
       <c r="J44" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3596,12 +3601,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L44" s="40" t="str">
-        <f>CONCATENATE("  {",I44,C44,", ",J44,K44,D44,", ",E44,"},")</f>
-        <v xml:space="preserve">  {"Btn 11 Mode", m_btn_mode, &amp;MenuValues[42], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 10 Mode", m_btn_mode, &amp;MenuValues[42], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M44" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 11 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 10 Mode</v>
       </c>
       <c r="N44" s="11"/>
     </row>
@@ -3611,7 +3616,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="20" t="s">
         <v>174</v>
@@ -3626,7 +3631,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A45,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[43]</v>
       </c>
       <c r="H45" s="29" t="s">
@@ -3634,7 +3639,7 @@
       </c>
       <c r="I45" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 12 Mode", </v>
+        <v xml:space="preserve">"Btn 11 Mode", </v>
       </c>
       <c r="J45" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3645,12 +3650,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L45" s="40" t="str">
-        <f>CONCATENATE("  {",I45,C45,", ",J45,K45,D45,", ",E45,"},")</f>
-        <v xml:space="preserve">  {"Btn 12 Mode", m_btn_mode, &amp;MenuValues[43], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 11 Mode", m_btn_mode, &amp;MenuValues[43], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M45" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 12 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 11 Mode</v>
       </c>
       <c r="N45" s="11"/>
     </row>
@@ -3660,7 +3665,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="20" t="s">
         <v>174</v>
@@ -3675,7 +3680,7 @@
         <v>0</v>
       </c>
       <c r="G46" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A46,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[44]</v>
       </c>
       <c r="H46" s="29" t="s">
@@ -3683,7 +3688,7 @@
       </c>
       <c r="I46" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 13 Mode", </v>
+        <v xml:space="preserve">"Btn 12 Mode", </v>
       </c>
       <c r="J46" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3694,12 +3699,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L46" s="40" t="str">
-        <f>CONCATENATE("  {",I46,C46,", ",J46,K46,D46,", ",E46,"},")</f>
-        <v xml:space="preserve">  {"Btn 13 Mode", m_btn_mode, &amp;MenuValues[44], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 12 Mode", m_btn_mode, &amp;MenuValues[44], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M46" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 13 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 12 Mode</v>
       </c>
       <c r="N46" s="11"/>
     </row>
@@ -3709,7 +3714,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="20" t="s">
         <v>174</v>
@@ -3724,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="G47" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A47,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[45]</v>
       </c>
       <c r="H47" s="29" t="s">
@@ -3732,7 +3737,7 @@
       </c>
       <c r="I47" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 14 Mode", </v>
+        <v xml:space="preserve">"Btn 13 Mode", </v>
       </c>
       <c r="J47" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3743,12 +3748,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L47" s="40" t="str">
-        <f>CONCATENATE("  {",I47,C47,", ",J47,K47,D47,", ",E47,"},")</f>
-        <v xml:space="preserve">  {"Btn 14 Mode", m_btn_mode, &amp;MenuValues[45], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 13 Mode", m_btn_mode, &amp;MenuValues[45], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M47" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 14 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 13 Mode</v>
       </c>
       <c r="N47" s="11"/>
     </row>
@@ -3758,7 +3763,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="20" t="s">
         <v>174</v>
@@ -3773,7 +3778,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A48,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[46]</v>
       </c>
       <c r="H48" s="29" t="s">
@@ -3781,7 +3786,7 @@
       </c>
       <c r="I48" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 15 Mode", </v>
+        <v xml:space="preserve">"Btn 14 Mode", </v>
       </c>
       <c r="J48" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3792,12 +3797,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L48" s="40" t="str">
-        <f>CONCATENATE("  {",I48,C48,", ",J48,K48,D48,", ",E48,"},")</f>
-        <v xml:space="preserve">  {"Btn 15 Mode", m_btn_mode, &amp;MenuValues[46], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 14 Mode", m_btn_mode, &amp;MenuValues[46], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M48" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 15 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 14 Mode</v>
       </c>
       <c r="N48" s="11"/>
     </row>
@@ -3807,7 +3812,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="20" t="s">
         <v>174</v>
@@ -3822,7 +3827,7 @@
         <v>0</v>
       </c>
       <c r="G49" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A49,"]")</f>
+        <f t="shared" si="14"/>
         <v>MenuValues[47]</v>
       </c>
       <c r="H49" s="29" t="s">
@@ -3830,7 +3835,7 @@
       </c>
       <c r="I49" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn 16 Mode", </v>
+        <v xml:space="preserve">"Btn 15 Mode", </v>
       </c>
       <c r="J49" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3841,12 +3846,12 @@
         <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L49" s="40" t="str">
-        <f>CONCATENATE("  {",I49,C49,", ",J49,K49,D49,", ",E49,"},")</f>
-        <v xml:space="preserve">  {"Btn 16 Mode", m_btn_mode, &amp;MenuValues[47], &amp;setBtnMode, 0, 3},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 15 Mode", m_btn_mode, &amp;MenuValues[47], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M49" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  0,  // Btn 16 Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 15 Mode</v>
       </c>
       <c r="N49" s="11"/>
     </row>
@@ -3855,46 +3860,47 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>177</v>
+      <c r="B50" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C50" s="20" t="s">
         <v>174</v>
       </c>
-      <c r="D50" s="61">
-        <v>-1</v>
-      </c>
-      <c r="E50" s="61">
-        <v>-1</v>
-      </c>
-      <c r="F50" s="61">
-        <v>-1</v>
-      </c>
-      <c r="G50" s="29" t="s">
-        <v>97</v>
+      <c r="D50" s="20">
+        <v>0</v>
+      </c>
+      <c r="E50" s="20">
+        <v>3</v>
+      </c>
+      <c r="F50" s="20">
+        <v>0</v>
+      </c>
+      <c r="G50" s="29" t="str">
+        <f t="shared" si="14"/>
+        <v>MenuValues[48]</v>
       </c>
       <c r="H50" s="29" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="I50" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Btn Mode", </v>
+        <v xml:space="preserve">"Btn 16 Mode", </v>
       </c>
       <c r="J50" s="44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">NULL, </v>
+        <v xml:space="preserve">&amp;MenuValues[48], </v>
       </c>
       <c r="K50" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
+        <v xml:space="preserve">&amp;setBtnMode, </v>
       </c>
       <c r="L50" s="40" t="str">
-        <f>CONCATENATE("  {",I50,C50,", ",J50,K50,D50,", ",E50,"},")</f>
-        <v xml:space="preserve">  {"Btn Mode", m_btn_mode, NULL, NULL, -1, -1},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn 16 Mode", m_btn_mode, &amp;MenuValues[48], &amp;setBtnMode, 0, 3},</v>
       </c>
       <c r="M50" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  -1,  // Btn Mode</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  0,  // Btn 16 Mode</v>
       </c>
       <c r="N50" s="11"/>
     </row>
@@ -3903,47 +3909,46 @@
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>4</v>
+      <c r="B51" s="13" t="s">
+        <v>177</v>
       </c>
       <c r="C51" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D51" s="30">
-        <v>0</v>
-      </c>
-      <c r="E51" s="12">
-        <v>4</v>
-      </c>
-      <c r="F51" s="30">
-        <v>1</v>
-      </c>
-      <c r="G51" s="29" t="str">
-        <f>CONCATENATE("MenuValues[",A51,"]")</f>
-        <v>MenuValues[49]</v>
+        <v>174</v>
+      </c>
+      <c r="D51" s="61">
+        <v>-1</v>
+      </c>
+      <c r="E51" s="61">
+        <v>-1</v>
+      </c>
+      <c r="F51" s="61">
+        <v>-1</v>
+      </c>
+      <c r="G51" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>178</v>
+        <v>97</v>
       </c>
       <c r="I51" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Kbd Driver", </v>
+        <v xml:space="preserve">"Btn Mode", </v>
       </c>
       <c r="J51" s="44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">&amp;MenuValues[49], </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="K51" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">&amp;setKbdDriver, </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L51" s="40" t="str">
-        <f>CONCATENATE("  {",I51,C51,", ",J51,K51,D51,", ",E51,"},")</f>
-        <v xml:space="preserve">  {"Kbd Driver", m_kbd_driver, &amp;MenuValues[49], &amp;setKbdDriver, 0, 4},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Btn Mode", m_btn_mode, NULL, NULL, -1, -1},</v>
       </c>
       <c r="M51" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  1,  // Kbd Driver</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  -1,  // Btn Mode</v>
       </c>
       <c r="N51" s="11"/>
     </row>
@@ -3952,31 +3957,31 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>5</v>
+      <c r="B52" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="C52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="30">
+        <v>0</v>
+      </c>
+      <c r="E52" s="12">
+        <v>4</v>
+      </c>
+      <c r="F52" s="30">
         <v>1</v>
-      </c>
-      <c r="E52" s="1">
-        <v>30</v>
-      </c>
-      <c r="F52" s="20">
-        <v>10</v>
       </c>
       <c r="G52" s="29" t="str">
         <f>CONCATENATE("MenuValues[",A52,"]")</f>
         <v>MenuValues[50]</v>
       </c>
-      <c r="H52" s="36" t="s">
-        <v>182</v>
+      <c r="H52" s="29" t="s">
+        <v>178</v>
       </c>
       <c r="I52" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Velocity Min", </v>
+        <v xml:space="preserve">"Kbd Driver", </v>
       </c>
       <c r="J52" s="44" t="str">
         <f t="shared" si="3"/>
@@ -3984,15 +3989,15 @@
       </c>
       <c r="K52" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">&amp;setDynSlope, </v>
+        <v xml:space="preserve">&amp;setKbdDriver, </v>
       </c>
       <c r="L52" s="40" t="str">
-        <f>CONCATENATE("  {",I52,C52,", ",J52,K52,D52,", ",E52,"},")</f>
-        <v xml:space="preserve">  {"Velocity Min", m_kbd_driver, &amp;MenuValues[50], &amp;setDynSlope, 1, 30},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Kbd Driver", m_kbd_driver, &amp;MenuValues[50], &amp;setKbdDriver, 0, 4},</v>
       </c>
       <c r="M52" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  10,  // Velocity Min</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  1,  // Kbd Driver</v>
       </c>
       <c r="N52" s="11"/>
     </row>
@@ -4002,16 +4007,16 @@
         <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C53" s="20" t="s">
         <v>112</v>
       </c>
       <c r="D53" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="F53" s="20">
         <v>10</v>
@@ -4020,12 +4025,12 @@
         <f>CONCATENATE("MenuValues[",A53,"]")</f>
         <v>MenuValues[51]</v>
       </c>
-      <c r="H53" s="29" t="s">
-        <v>97</v>
+      <c r="H53" s="36" t="s">
+        <v>182</v>
       </c>
       <c r="I53" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Velocity MaxAdj", </v>
+        <v xml:space="preserve">"Velocity Min", </v>
       </c>
       <c r="J53" s="44" t="str">
         <f t="shared" si="3"/>
@@ -4033,15 +4038,15 @@
       </c>
       <c r="K53" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">NULL, </v>
+        <v xml:space="preserve">&amp;setDynSlope, </v>
       </c>
       <c r="L53" s="40" t="str">
-        <f>CONCATENATE("  {",I53,C53,", ",J53,K53,D53,", ",E53,"},")</f>
-        <v xml:space="preserve">  {"Velocity MaxAdj", m_kbd_driver, &amp;MenuValues[51], NULL, 0, 20},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Velocity Min", m_kbd_driver, &amp;MenuValues[51], &amp;setDynSlope, 1, 30},</v>
       </c>
       <c r="M53" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  10,  // Velocity MaxAdj</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  10,  // Velocity Min</v>
       </c>
       <c r="N53" s="11"/>
     </row>
@@ -4051,30 +4056,30 @@
         <v>52</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C54" s="20" t="s">
         <v>112</v>
       </c>
       <c r="D54" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F54" s="20">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G54" s="29" t="str">
         <f>CONCATENATE("MenuValues[",A54,"]")</f>
         <v>MenuValues[52]</v>
       </c>
-      <c r="H54" s="36" t="s">
-        <v>182</v>
+      <c r="H54" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="I54" s="43" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">"Velocity Slope", </v>
+        <v xml:space="preserve">"Velocity MaxAdj", </v>
       </c>
       <c r="J54" s="44" t="str">
         <f t="shared" si="3"/>
@@ -4082,74 +4087,74 @@
       </c>
       <c r="K54" s="44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">&amp;setDynSlope, </v>
+        <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L54" s="40" t="str">
-        <f>CONCATENATE("  {",I54,C54,", ",J54,K54,D54,", ",E54,"},")</f>
-        <v xml:space="preserve">  {"Velocity Slope", m_kbd_driver, &amp;MenuValues[52], &amp;setDynSlope, 1, 40},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Velocity MaxAdj", m_kbd_driver, &amp;MenuValues[52], NULL, 0, 20},</v>
       </c>
       <c r="M54" s="76" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">  20,  // Velocity Slope</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  10,  // Velocity MaxAdj</v>
       </c>
       <c r="N54" s="11"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="21">
-        <f t="shared" ref="A55:A58" si="7">A54+1</f>
+        <f t="shared" si="1"/>
         <v>53</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C55" s="20" t="s">
         <v>112</v>
       </c>
       <c r="D55" s="20">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F55" s="20">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="G55" s="29" t="str">
-        <f t="shared" ref="G55:G59" si="8">CONCATENATE("MenuValues[",A55,"]")</f>
+        <f>CONCATENATE("MenuValues[",A55,"]")</f>
         <v>MenuValues[53]</v>
       </c>
-      <c r="H55" s="29" t="s">
-        <v>97</v>
+      <c r="H55" s="36" t="s">
+        <v>182</v>
       </c>
       <c r="I55" s="43" t="str">
-        <f t="shared" ref="I55:I58" si="9">CONCATENATE("""",B55,""", ")</f>
-        <v xml:space="preserve">"Upper Base", </v>
+        <f t="shared" si="2"/>
+        <v xml:space="preserve">"Velocity Slope", </v>
       </c>
       <c r="J55" s="44" t="str">
-        <f t="shared" ref="J55:J58" si="10">IF(G55="NULL",CONCATENATE(G55,", "),CONCATENATE("&amp;",G55,", "))</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">&amp;MenuValues[53], </v>
       </c>
       <c r="K55" s="44" t="str">
-        <f t="shared" ref="K55:K58" si="11">IF(H55="NULL",CONCATENATE(H55,", "),CONCATENATE("&amp;",H55,", "))</f>
-        <v xml:space="preserve">NULL, </v>
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">&amp;setDynSlope, </v>
       </c>
       <c r="L55" s="40" t="str">
-        <f t="shared" ref="L55:L58" si="12">CONCATENATE("  {",I55,C55,", ",J55,K55,D55,", ",E55,"},")</f>
-        <v xml:space="preserve">  {"Upper Base", m_kbd_driver, &amp;MenuValues[53], NULL, 12, 60},</v>
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">  {"Velocity Slope", m_kbd_driver, &amp;MenuValues[53], &amp;setDynSlope, 1, 40},</v>
       </c>
       <c r="M55" s="76" t="str">
-        <f t="shared" ref="M55:M58" si="13" xml:space="preserve"> CONCATENATE("  ",F55,",  // ",B55)</f>
-        <v xml:space="preserve">  36,  // Upper Base</v>
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">  20,  // Velocity Slope</v>
       </c>
       <c r="N55" s="11"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A56:A59" si="16">A55+1</f>
         <v>54</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56" s="20" t="s">
         <v>112</v>
@@ -4164,40 +4169,41 @@
         <v>36</v>
       </c>
       <c r="G56" s="29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="G56:G59" si="17">CONCATENATE("MenuValues[",A56,"]")</f>
         <v>MenuValues[54]</v>
       </c>
       <c r="H56" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I56" s="43" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">"Lower Base", </v>
+        <f t="shared" ref="I56:I59" si="18">CONCATENATE("""",B56,""", ")</f>
+        <v xml:space="preserve">"Upper Base", </v>
       </c>
       <c r="J56" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="J56:J59" si="19">IF(G56="NULL",CONCATENATE(G56,", "),CONCATENATE("&amp;",G56,", "))</f>
         <v xml:space="preserve">&amp;MenuValues[54], </v>
       </c>
       <c r="K56" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="K56:K59" si="20">IF(H56="NULL",CONCATENATE(H56,", "),CONCATENATE("&amp;",H56,", "))</f>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L56" s="40" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">  {"Lower Base", m_kbd_driver, &amp;MenuValues[54], NULL, 12, 60},</v>
+        <f t="shared" ref="L56:L59" si="21">CONCATENATE("  {",I56,C56,", ",J56,K56,D56,", ",E56,"},")</f>
+        <v xml:space="preserve">  {"Upper Base", m_kbd_driver, &amp;MenuValues[54], NULL, 12, 60},</v>
       </c>
       <c r="M56" s="76" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">  36,  // Lower Base</v>
-      </c>
+        <f t="shared" ref="M56:M59" si="22" xml:space="preserve"> CONCATENATE("  ",F56,",  // ",B56)</f>
+        <v xml:space="preserve">  36,  // Upper Base</v>
+      </c>
+      <c r="N56" s="11"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>55</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="20" t="s">
         <v>112</v>
@@ -4212,127 +4218,149 @@
         <v>36</v>
       </c>
       <c r="G57" s="29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>MenuValues[55]</v>
       </c>
       <c r="H57" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I57" s="43" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve">"Pedal Base", </v>
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">"Lower Base", </v>
       </c>
       <c r="J57" s="44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">&amp;MenuValues[55], </v>
       </c>
       <c r="K57" s="44" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="20"/>
         <v xml:space="preserve">NULL, </v>
       </c>
       <c r="L57" s="40" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">  {"Pedal Base", m_kbd_driver, &amp;MenuValues[55], NULL, 12, 60},</v>
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  {"Lower Base", m_kbd_driver, &amp;MenuValues[55], NULL, 12, 60},</v>
       </c>
       <c r="M57" s="76" t="str">
-        <f t="shared" si="13"/>
-        <v xml:space="preserve">  36,  // Pedal Base</v>
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">  36,  // Lower Base</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="16"/>
         <v>56</v>
       </c>
-      <c r="B58" s="13" t="s">
-        <v>25</v>
+      <c r="B58" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C58" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="D58" s="61">
-        <v>-1</v>
-      </c>
-      <c r="E58" s="61">
-        <v>-1</v>
-      </c>
-      <c r="F58" s="61">
-        <v>-1</v>
+      <c r="D58" s="20">
+        <v>12</v>
+      </c>
+      <c r="E58" s="1">
+        <v>60</v>
+      </c>
+      <c r="F58" s="20">
+        <v>36</v>
       </c>
       <c r="G58" s="29" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="17"/>
         <v>MenuValues[56]</v>
       </c>
       <c r="H58" s="29" t="s">
         <v>97</v>
       </c>
       <c r="I58" s="43" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="18"/>
+        <v xml:space="preserve">"Pedal Base", </v>
+      </c>
+      <c r="J58" s="44" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">&amp;MenuValues[56], </v>
+      </c>
+      <c r="K58" s="44" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L58" s="40" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  {"Pedal Base", m_kbd_driver, &amp;MenuValues[56], NULL, 12, 60},</v>
+      </c>
+      <c r="M58" s="76" t="str">
+        <f t="shared" si="22"/>
+        <v xml:space="preserve">  36,  // Pedal Base</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="21">
+        <f t="shared" si="16"/>
+        <v>57</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="61">
+        <v>-1</v>
+      </c>
+      <c r="E59" s="61">
+        <v>-1</v>
+      </c>
+      <c r="F59" s="61">
+        <v>-1</v>
+      </c>
+      <c r="G59" s="29" t="str">
+        <f t="shared" si="17"/>
+        <v>MenuValues[57]</v>
+      </c>
+      <c r="H59" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="I59" s="43" t="str">
+        <f t="shared" si="18"/>
         <v xml:space="preserve">"Keyboard", </v>
       </c>
-      <c r="J58" s="44" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve">&amp;MenuValues[56], </v>
-      </c>
-      <c r="K58" s="44" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve">NULL, </v>
-      </c>
-      <c r="L58" s="40" t="str">
-        <f t="shared" si="12"/>
-        <v xml:space="preserve">  {"Keyboard", m_kbd_driver, &amp;MenuValues[56], NULL, -1, -1},</v>
-      </c>
-      <c r="M58" s="76" t="str">
-        <f t="shared" si="13"/>
+      <c r="J59" s="44" t="str">
+        <f t="shared" si="19"/>
+        <v xml:space="preserve">&amp;MenuValues[57], </v>
+      </c>
+      <c r="K59" s="44" t="str">
+        <f t="shared" si="20"/>
+        <v xml:space="preserve">NULL, </v>
+      </c>
+      <c r="L59" s="40" t="str">
+        <f t="shared" si="21"/>
+        <v xml:space="preserve">  {"Keyboard", m_kbd_driver, &amp;MenuValues[57], NULL, -1, -1},</v>
+      </c>
+      <c r="M59" s="76" t="str">
+        <f t="shared" si="22"/>
         <v xml:space="preserve">  -1,  // Keyboard</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="77">
-        <f>A58+1</f>
-        <v>57</v>
-      </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="20"/>
-      <c r="I59" s="10"/>
-      <c r="J59" s="9" t="s">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="77">
+        <f>A59+1</f>
+        <v>58</v>
+      </c>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K59" s="1" t="s">
+      <c r="K60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L59" s="40" t="s">
+      <c r="L60" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="M59" s="39" t="s">
+      <c r="M60" s="39" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="73" t="s">
-        <v>164</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C60" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="D60" s="61">
-        <v>-1</v>
-      </c>
-      <c r="E60" s="61">
-        <v>-1</v>
-      </c>
-      <c r="F60" s="61"/>
-      <c r="G60" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="J60" s="10"/>
-      <c r="L60" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="M60" s="76"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="73" t="s">
@@ -4344,92 +4372,118 @@
       <c r="C61" s="68" t="s">
         <v>162</v>
       </c>
-      <c r="D61" s="70">
-        <v>0</v>
-      </c>
-      <c r="E61" s="70">
-        <v>0</v>
-      </c>
-      <c r="F61" s="70"/>
+      <c r="D61" s="61">
+        <v>-1</v>
+      </c>
+      <c r="E61" s="61">
+        <v>-1</v>
+      </c>
+      <c r="F61" s="61"/>
       <c r="G61" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="J61" s="10"/>
+      <c r="L61" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="M61" s="76"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="73" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C62" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="D62" s="70">
+        <v>0</v>
+      </c>
+      <c r="E62" s="70">
+        <v>0</v>
+      </c>
+      <c r="F62" s="70"/>
+      <c r="G62" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="L61" s="74" t="str">
-        <f>CONCATENATE("#define MENU_POT_CC ",A12)</f>
-        <v>#define MENU_POT_CC 10</v>
-      </c>
-      <c r="M61" s="76"/>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G62" s="39" t="str">
-        <f>CONCATENATE("#define MENU_ITEMCOUNT ",A59)</f>
-        <v>#define MENU_ITEMCOUNT 57</v>
-      </c>
-      <c r="H62" s="39"/>
-      <c r="I62" s="6" t="s">
+      <c r="L62" s="74" t="str">
+        <f>CONCATENATE("#define MENU_POT_CC ",A13)</f>
+        <v>#define MENU_POT_CC 11</v>
+      </c>
+      <c r="M62" s="76"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G63" s="39" t="str">
+        <f>CONCATENATE("#define MENU_ITEMCOUNT ",A60)</f>
+        <v>#define MENU_ITEMCOUNT 58</v>
+      </c>
+      <c r="H63" s="39"/>
+      <c r="I63" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="L62" s="74" t="str">
-        <f>CONCATENATE("#define MENU_BTN_CC ",A17)</f>
-        <v>#define MENU_BTN_CC 15</v>
-      </c>
-      <c r="M62" s="76"/>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L63" s="74" t="str">
-        <f>CONCATENATE("#define MENU_BTN_MODE ",A34)</f>
-        <v>#define MENU_BTN_MODE 32</v>
+        <f>CONCATENATE("#define MENU_BTN_CC ",A18)</f>
+        <v>#define MENU_BTN_CC 16</v>
       </c>
       <c r="M63" s="76"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L64" s="74" t="str">
-        <f>CONCATENATE("#define MENU_KBD_DRIVER ",A51)</f>
-        <v>#define MENU_KBD_DRIVER 49</v>
+        <f>CONCATENATE("#define MENU_BTN_MODE ",A35)</f>
+        <v>#define MENU_BTN_MODE 33</v>
       </c>
       <c r="M64" s="76"/>
     </row>
     <row r="65" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L65" s="74" t="str">
-        <f>CONCATENATE("#define MENU_MIN_DYN ",A52)</f>
-        <v>#define MENU_MIN_DYN 50</v>
+        <f>CONCATENATE("#define MENU_KBD_DRIVER ",A52)</f>
+        <v>#define MENU_KBD_DRIVER 50</v>
       </c>
       <c r="M65" s="76"/>
     </row>
     <row r="66" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L66" s="74" t="str">
-        <f>CONCATENATE("#define MENU_MAX_DYNADJ ",A53)</f>
-        <v>#define MENU_MAX_DYNADJ 51</v>
+        <f>CONCATENATE("#define MENU_MIN_DYN ",A53)</f>
+        <v>#define MENU_MIN_DYN 51</v>
       </c>
       <c r="M66" s="76"/>
     </row>
     <row r="67" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L67" s="74" t="str">
-        <f>CONCATENATE("#define MENU_DYNSLOPE ",A54)</f>
-        <v>#define MENU_DYNSLOPE 52</v>
+        <f>CONCATENATE("#define MENU_MAX_DYNADJ ",A54)</f>
+        <v>#define MENU_MAX_DYNADJ 52</v>
       </c>
       <c r="M67" s="76"/>
     </row>
     <row r="68" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L68" s="74" t="str">
-        <f>CONCATENATE("#define MENU_BASE_UPR ",A55)</f>
-        <v>#define MENU_BASE_UPR 53</v>
+        <f>CONCATENATE("#define MENU_DYNSLOPE ",A55)</f>
+        <v>#define MENU_DYNSLOPE 53</v>
       </c>
       <c r="M68" s="76"/>
     </row>
     <row r="69" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L69" s="74" t="str">
-        <f>CONCATENATE("#define MENU_BASE_LWR ",A56)</f>
-        <v>#define MENU_BASE_LWR 54</v>
+        <f>CONCATENATE("#define MENU_BASE_UPR ",A56)</f>
+        <v>#define MENU_BASE_UPR 54</v>
       </c>
       <c r="M69" s="76"/>
     </row>
     <row r="70" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L70" s="74" t="str">
-        <f>CONCATENATE("#define MENU_BASE_PED ",A57)</f>
-        <v>#define MENU_BASE_PED 55</v>
+        <f>CONCATENATE("#define MENU_BASE_LWR ",A57)</f>
+        <v>#define MENU_BASE_LWR 55</v>
       </c>
       <c r="M70" s="76"/>
+    </row>
+    <row r="71" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L71" s="74" t="str">
+        <f>CONCATENATE("#define MENU_BASE_PED ",A58)</f>
+        <v>#define MENU_BASE_PED 56</v>
+      </c>
+      <c r="M71" s="76"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>